<commit_message>
Message 325321977385069 - 1760977492
</commit_message>
<xml_diff>
--- a/user_input_files/planillas-web/Fuentes_Poder.xlsx
+++ b/user_input_files/planillas-web/Fuentes_Poder.xlsx
@@ -7,14 +7,14 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="Fuentes_Poder" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="68">
   <si>
     <t>ID Fuente</t>
   </si>
@@ -55,6 +55,18 @@
     <t>Observaciones</t>
   </si>
   <si>
+    <t>Tipo</t>
+  </si>
+  <si>
+    <t>Marca</t>
+  </si>
+  <si>
+    <t>Voltaje Salida (V)</t>
+  </si>
+  <si>
+    <t>Gabinete Asociado</t>
+  </si>
+  <si>
     <t>FP-001</t>
   </si>
   <si>
@@ -64,6 +76,24 @@
     <t>FP-003</t>
   </si>
   <si>
+    <t>FP-004</t>
+  </si>
+  <si>
+    <t>FP-005</t>
+  </si>
+  <si>
+    <t>FP-006</t>
+  </si>
+  <si>
+    <t>UBI-006</t>
+  </si>
+  <si>
+    <t>UBI-007</t>
+  </si>
+  <si>
+    <t>UBI-004</t>
+  </si>
+  <si>
     <t>Meanwell RS-150-12</t>
   </si>
   <si>
@@ -73,6 +103,15 @@
     <t>Meanwell RS-100-12</t>
   </si>
   <si>
+    <t>PS-1205</t>
+  </si>
+  <si>
+    <t>PS-1210-R</t>
+  </si>
+  <si>
+    <t>PS-1203</t>
+  </si>
+  <si>
     <t>Switch GAB-O-P3</t>
   </si>
   <si>
@@ -82,6 +121,15 @@
     <t>Switch CFT Prat</t>
   </si>
   <si>
+    <t>3 cámaras bullet</t>
+  </si>
+  <si>
+    <t>Respaldo para cámaras no-PoE</t>
+  </si>
+  <si>
+    <t>2 cámaras AHD</t>
+  </si>
+  <si>
     <t>GAB-O-P3</t>
   </si>
   <si>
@@ -106,6 +154,9 @@
     <t>Operativo</t>
   </si>
   <si>
+    <t>Activo</t>
+  </si>
+  <si>
     <t>2023-03-15</t>
   </si>
   <si>
@@ -115,6 +166,15 @@
     <t>2023-05-20</t>
   </si>
   <si>
+    <t>2024-08-05</t>
+  </si>
+  <si>
+    <t>2024-05-12</t>
+  </si>
+  <si>
+    <t>2024-06-20</t>
+  </si>
+  <si>
     <t>Fuente original del sistema</t>
   </si>
   <si>
@@ -122,6 +182,42 @@
   </si>
   <si>
     <t>Funcionando correctamente</t>
+  </si>
+  <si>
+    <t>Fuente externa gabinete Pucón</t>
+  </si>
+  <si>
+    <t>Fuente redundante CFT Prat</t>
+  </si>
+  <si>
+    <t>Alimentación cámaras analógicas</t>
+  </si>
+  <si>
+    <t>Fuente 12V 5A</t>
+  </si>
+  <si>
+    <t>Fuente 12V 10A</t>
+  </si>
+  <si>
+    <t>Fuente 12V 3A</t>
+  </si>
+  <si>
+    <t>PowerTech</t>
+  </si>
+  <si>
+    <t>Altronix</t>
+  </si>
+  <si>
+    <t>Generic</t>
+  </si>
+  <si>
+    <t>GAB-004</t>
+  </si>
+  <si>
+    <t>GAB-005</t>
+  </si>
+  <si>
+    <t>GAB-006</t>
   </si>
 </sst>
 </file>
@@ -479,13 +575,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M4"/>
+  <dimension ref="A1:Q7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:17">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -525,13 +621,25 @@
       <c r="M1" s="1" t="s">
         <v>12</v>
       </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="2" spans="1:13">
+    <row r="2" spans="1:17">
       <c r="A2" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="C2" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="D2">
         <v>12</v>
@@ -543,33 +651,33 @@
         <v>150</v>
       </c>
       <c r="G2" t="s">
-        <v>19</v>
+        <v>32</v>
       </c>
       <c r="H2" t="s">
-        <v>22</v>
+        <v>38</v>
       </c>
       <c r="I2" t="s">
-        <v>25</v>
+        <v>41</v>
       </c>
       <c r="J2" t="s">
-        <v>28</v>
+        <v>44</v>
       </c>
       <c r="K2" t="s">
-        <v>29</v>
+        <v>45</v>
       </c>
       <c r="L2" t="s">
-        <v>30</v>
+        <v>47</v>
       </c>
       <c r="M2" t="s">
-        <v>33</v>
+        <v>53</v>
       </c>
     </row>
-    <row r="3" spans="1:13">
+    <row r="3" spans="1:17">
       <c r="A3" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="C3" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="D3">
         <v>12</v>
@@ -581,33 +689,33 @@
         <v>60</v>
       </c>
       <c r="G3" t="s">
-        <v>20</v>
+        <v>33</v>
       </c>
       <c r="H3" t="s">
-        <v>23</v>
+        <v>39</v>
       </c>
       <c r="I3" t="s">
-        <v>26</v>
+        <v>42</v>
       </c>
       <c r="J3" t="s">
+        <v>44</v>
+      </c>
+      <c r="K3" t="s">
+        <v>45</v>
+      </c>
+      <c r="L3" t="s">
+        <v>48</v>
+      </c>
+      <c r="M3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17">
+      <c r="A4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" t="s">
         <v>28</v>
-      </c>
-      <c r="K3" t="s">
-        <v>29</v>
-      </c>
-      <c r="L3" t="s">
-        <v>31</v>
-      </c>
-      <c r="M3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13">
-      <c r="A4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" t="s">
-        <v>18</v>
       </c>
       <c r="D4">
         <v>12</v>
@@ -619,25 +727,148 @@
         <v>100</v>
       </c>
       <c r="G4" t="s">
+        <v>34</v>
+      </c>
+      <c r="H4" t="s">
+        <v>40</v>
+      </c>
+      <c r="I4" t="s">
+        <v>43</v>
+      </c>
+      <c r="J4" t="s">
+        <v>44</v>
+      </c>
+      <c r="K4" t="s">
+        <v>45</v>
+      </c>
+      <c r="L4" t="s">
+        <v>49</v>
+      </c>
+      <c r="M4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17">
+      <c r="A5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" t="s">
+        <v>29</v>
+      </c>
+      <c r="E5">
+        <v>5</v>
+      </c>
+      <c r="F5">
+        <v>60</v>
+      </c>
+      <c r="G5" t="s">
+        <v>35</v>
+      </c>
+      <c r="K5" t="s">
+        <v>46</v>
+      </c>
+      <c r="L5" t="s">
+        <v>50</v>
+      </c>
+      <c r="M5" t="s">
+        <v>56</v>
+      </c>
+      <c r="N5" t="s">
+        <v>59</v>
+      </c>
+      <c r="O5" t="s">
+        <v>62</v>
+      </c>
+      <c r="P5">
+        <v>12</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17">
+      <c r="A6" t="s">
         <v>21</v>
       </c>
-      <c r="H4" t="s">
+      <c r="B6" t="s">
         <v>24</v>
       </c>
-      <c r="I4" t="s">
-        <v>27</v>
-      </c>
-      <c r="J4" t="s">
-        <v>28</v>
-      </c>
-      <c r="K4" t="s">
-        <v>29</v>
-      </c>
-      <c r="L4" t="s">
-        <v>32</v>
-      </c>
-      <c r="M4" t="s">
-        <v>35</v>
+      <c r="C6" t="s">
+        <v>30</v>
+      </c>
+      <c r="E6">
+        <v>10</v>
+      </c>
+      <c r="F6">
+        <v>120</v>
+      </c>
+      <c r="G6" t="s">
+        <v>36</v>
+      </c>
+      <c r="K6" t="s">
+        <v>46</v>
+      </c>
+      <c r="L6" t="s">
+        <v>51</v>
+      </c>
+      <c r="M6" t="s">
+        <v>57</v>
+      </c>
+      <c r="N6" t="s">
+        <v>60</v>
+      </c>
+      <c r="O6" t="s">
+        <v>63</v>
+      </c>
+      <c r="P6">
+        <v>12</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17">
+      <c r="A7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" t="s">
+        <v>31</v>
+      </c>
+      <c r="E7">
+        <v>3</v>
+      </c>
+      <c r="F7">
+        <v>36</v>
+      </c>
+      <c r="G7" t="s">
+        <v>37</v>
+      </c>
+      <c r="K7" t="s">
+        <v>46</v>
+      </c>
+      <c r="L7" t="s">
+        <v>52</v>
+      </c>
+      <c r="M7" t="s">
+        <v>58</v>
+      </c>
+      <c r="N7" t="s">
+        <v>61</v>
+      </c>
+      <c r="O7" t="s">
+        <v>64</v>
+      </c>
+      <c r="P7">
+        <v>12</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>